<commit_message>
Updated BOM to uniformize with other Harp boards.
</commit_message>
<xml_diff>
--- a/Hardware/PCB/harp behavior poke port breakout v2.1_BOM.xlsx
+++ b/Hardware/PCB/harp behavior poke port breakout v2.1_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_behavior\PCB modules\Port Breakout\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\production files\harp\OEPS-2205 - Harp Behavior - Breakout V2\pcb\v2.1\production files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B678742-5956-43F3-8B1F-236FF04CD807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FC20C7-C45D-4B72-8BB8-8BE1B7F186B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17895" yWindow="3210" windowWidth="7500" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Licensed under the TAPR Open Hardware License (www.tapr.org/OHL)</t>
   </si>
   <si>
-    <t>Copyright 2018 Artur Silva and Filipe Carvalho</t>
-  </si>
-  <si>
     <t>LP5907MFX-3.3/NOPB</t>
   </si>
   <si>
@@ -89,12 +86,6 @@
     <t>RES SMD 0402 1kΩ ±1% 62.5mW</t>
   </si>
   <si>
-    <t>RC0402FR-071KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-07100KL</t>
-  </si>
-  <si>
     <t>RES SMD 0402 100kΩ ±1% 62.5mW</t>
   </si>
   <si>
@@ -104,18 +95,12 @@
     <t>C1, C2</t>
   </si>
   <si>
-    <t>EMK107ABJ475KA-T</t>
-  </si>
-  <si>
     <t>CAP CER 0402 100nF 25V ±10% X7R</t>
   </si>
   <si>
     <t>C3</t>
   </si>
   <si>
-    <t>TMK105B7104KVHF</t>
-  </si>
-  <si>
     <t>SV1</t>
   </si>
   <si>
@@ -150,6 +135,21 @@
   </si>
   <si>
     <t>Single Schmitt-Trigger inverter buffer</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1001X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1003X</t>
+  </si>
+  <si>
+    <t>C1608X6S1C475K080AC</t>
+  </si>
+  <si>
+    <t>GRM155R71E104KE14D</t>
+  </si>
+  <si>
+    <t>Copyright 2020-2023 Artur Silva and Filipe Carvalho</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -690,9 +690,6 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1080,9 +1077,9 @@
   </sheetPr>
   <dimension ref="B1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1089,7 @@
     <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="70.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1111,7 +1108,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1127,7 +1124,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -1143,135 +1140,135 @@
         <v>7</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7">
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7">
         <v>1</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>1</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>1</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>20</v>
+      <c r="D9" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="7">
         <v>2</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>23</v>
+      <c r="D10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>26</v>
+      <c r="D11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
@@ -1303,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1321,7 +1318,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -1345,7 +1342,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>